<commit_message>
Update Vokabeltrainer Product Backlog.xlsx
</commit_message>
<xml_diff>
--- a/Vokabeltrainer Product Backlog.xlsx
+++ b/Vokabeltrainer Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claus\Documents\Schule\Scrum\Projekte\Vokabeltrainer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adria\Documents\.Workspace_Adrian_Java\Vokabeltrainer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8CF85D-BE34-45AA-8F66-DD80AE135D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7759CB-CB92-42BE-8D91-DD849B547D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vokabeltrainer" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -702,28 +700,28 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.7109375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="40.73046875" style="10" customWidth="1"/>
+    <col min="8" max="8" width="25.73046875" style="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.265625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="10.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -764,7 +762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>22</v>
       </c>
@@ -788,7 +786,7 @@
       <c r="L2" s="20"/>
       <c r="M2" s="20"/>
     </row>
-    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -812,7 +810,7 @@
       <c r="L3" s="23"/>
       <c r="M3" s="23"/>
     </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
@@ -825,7 +823,9 @@
       <c r="D4" s="13">
         <v>1</v>
       </c>
-      <c r="E4" s="14"/>
+      <c r="E4" s="14">
+        <v>13</v>
+      </c>
       <c r="F4" s="14"/>
       <c r="G4" s="15"/>
       <c r="H4" s="16"/>
@@ -835,7 +835,7 @@
       <c r="L4" s="14"/>
       <c r="M4" s="14"/>
     </row>
-    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A5" s="26" t="s">
         <v>14</v>
       </c>
@@ -848,7 +848,9 @@
       <c r="D5" s="13">
         <v>3</v>
       </c>
-      <c r="E5" s="14"/>
+      <c r="E5" s="14">
+        <v>5</v>
+      </c>
       <c r="F5" s="14"/>
       <c r="G5" s="15"/>
       <c r="H5" s="16"/>
@@ -858,7 +860,7 @@
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A6" s="26" t="s">
         <v>26</v>
       </c>
@@ -871,7 +873,9 @@
       <c r="D6" s="13">
         <v>3</v>
       </c>
-      <c r="E6" s="14"/>
+      <c r="E6" s="14">
+        <v>5</v>
+      </c>
       <c r="F6" s="14"/>
       <c r="G6" s="15"/>
       <c r="H6" s="16"/>
@@ -881,7 +885,7 @@
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
     </row>
-    <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>27</v>
       </c>
@@ -894,7 +898,9 @@
       <c r="D7" s="13">
         <v>2</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E7" s="14">
+        <v>2</v>
+      </c>
       <c r="F7" s="14"/>
       <c r="G7" s="15"/>
       <c r="H7" s="16"/>
@@ -904,7 +910,7 @@
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
     </row>
-    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8" s="26" t="s">
         <v>28</v>
       </c>
@@ -917,7 +923,9 @@
       <c r="D8" s="13">
         <v>3</v>
       </c>
-      <c r="E8" s="14"/>
+      <c r="E8" s="14">
+        <v>3</v>
+      </c>
       <c r="F8" s="14"/>
       <c r="G8" s="15"/>
       <c r="H8" s="16"/>
@@ -927,7 +935,7 @@
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>47</v>
       </c>
@@ -940,7 +948,9 @@
       <c r="D9" s="13">
         <v>3</v>
       </c>
-      <c r="E9" s="14"/>
+      <c r="E9" s="14">
+        <v>1</v>
+      </c>
       <c r="F9" s="14"/>
       <c r="G9" s="15"/>
       <c r="H9" s="16"/>
@@ -950,7 +960,7 @@
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
     </row>
-    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -974,7 +984,7 @@
       <c r="L10" s="23"/>
       <c r="M10" s="23"/>
     </row>
-    <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>16</v>
       </c>
@@ -987,7 +997,9 @@
       <c r="D11" s="13">
         <v>1</v>
       </c>
-      <c r="E11" s="14"/>
+      <c r="E11" s="14">
+        <v>8</v>
+      </c>
       <c r="F11" s="14"/>
       <c r="G11" s="15"/>
       <c r="H11" s="16"/>
@@ -997,7 +1009,7 @@
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
     </row>
-    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>17</v>
       </c>
@@ -1010,7 +1022,9 @@
       <c r="D12" s="13">
         <v>2</v>
       </c>
-      <c r="E12" s="14"/>
+      <c r="E12" s="14">
+        <v>1</v>
+      </c>
       <c r="F12" s="14"/>
       <c r="G12" s="15"/>
       <c r="H12" s="16"/>
@@ -1020,7 +1034,7 @@
       <c r="L12" s="14"/>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>18</v>
       </c>
@@ -1033,7 +1047,9 @@
       <c r="D13" s="13">
         <v>2</v>
       </c>
-      <c r="E13" s="14"/>
+      <c r="E13" s="14">
+        <v>3</v>
+      </c>
       <c r="F13" s="14"/>
       <c r="G13" s="15"/>
       <c r="H13" s="16"/>
@@ -1043,7 +1059,7 @@
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
     </row>
-    <row r="14" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>19</v>
       </c>
@@ -1056,7 +1072,9 @@
       <c r="D14" s="13">
         <v>2</v>
       </c>
-      <c r="E14" s="14"/>
+      <c r="E14" s="14">
+        <v>5</v>
+      </c>
       <c r="F14" s="14"/>
       <c r="G14" s="15"/>
       <c r="H14" s="16"/>
@@ -1066,7 +1084,7 @@
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>29</v>
       </c>
@@ -1079,7 +1097,9 @@
       <c r="D15" s="13">
         <v>3</v>
       </c>
-      <c r="E15" s="14"/>
+      <c r="E15" s="14">
+        <v>3</v>
+      </c>
       <c r="F15" s="14"/>
       <c r="G15" s="15"/>
       <c r="H15" s="16"/>
@@ -1089,7 +1109,7 @@
       <c r="L15" s="14"/>
       <c r="M15" s="14"/>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>30</v>
       </c>
@@ -1102,7 +1122,9 @@
       <c r="D16" s="13">
         <v>3</v>
       </c>
-      <c r="E16" s="14"/>
+      <c r="E16" s="14">
+        <v>2</v>
+      </c>
       <c r="F16" s="14"/>
       <c r="G16" s="15"/>
       <c r="H16" s="16"/>
@@ -1112,7 +1134,7 @@
       <c r="L16" s="14"/>
       <c r="M16" s="14"/>
     </row>
-    <row r="17" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>31</v>
       </c>
@@ -1125,7 +1147,9 @@
       <c r="D17" s="13">
         <v>1</v>
       </c>
-      <c r="E17" s="14"/>
+      <c r="E17" s="14">
+        <v>8</v>
+      </c>
       <c r="F17" s="14"/>
       <c r="G17" s="15"/>
       <c r="H17" s="16"/>
@@ -1135,7 +1159,7 @@
       <c r="L17" s="14"/>
       <c r="M17" s="14"/>
     </row>
-    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>32</v>
       </c>
@@ -1148,7 +1172,9 @@
       <c r="D18" s="13">
         <v>1</v>
       </c>
-      <c r="E18" s="14"/>
+      <c r="E18" s="14">
+        <v>5</v>
+      </c>
       <c r="F18" s="14"/>
       <c r="G18" s="15"/>
       <c r="H18" s="16"/>
@@ -1158,7 +1184,7 @@
       <c r="L18" s="14"/>
       <c r="M18" s="14"/>
     </row>
-    <row r="19" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="57" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
         <v>52</v>
       </c>
@@ -1171,7 +1197,9 @@
       <c r="D19" s="13">
         <v>3</v>
       </c>
-      <c r="E19" s="14"/>
+      <c r="E19" s="14">
+        <v>5</v>
+      </c>
       <c r="F19" s="14"/>
       <c r="G19" s="15"/>
       <c r="H19" s="16"/>
@@ -1181,7 +1209,7 @@
       <c r="L19" s="14"/>
       <c r="M19" s="14"/>
     </row>
-    <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>53</v>
       </c>
@@ -1194,7 +1222,9 @@
       <c r="D20" s="13">
         <v>3</v>
       </c>
-      <c r="E20" s="14"/>
+      <c r="E20" s="14">
+        <v>3</v>
+      </c>
       <c r="F20" s="14"/>
       <c r="G20" s="15"/>
       <c r="H20" s="16"/>
@@ -1217,7 +1247,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:M20">
     <sortCondition ref="A3:A20"/>
   </sortState>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="ungültige Eingabe" error="Markieren Sie mit einem X, welchen Status diese Anforderung hat." sqref="I3:M20" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"X"</formula1>
     </dataValidation>

</xml_diff>